<commit_message>
Added spreadsheeting capability. Also split retirement year so that contributions and withdrawals only happen for appropriate months, and RA lump sum is paid at retirement month
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,15 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">Financial Year</t>
+    <t xml:space="preserve">Financial year</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly IBT</t>
@@ -44,11 +44,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -65,6 +67,14 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -74,12 +84,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -108,9 +125,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -130,41 +151,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>2019</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -180,8 +201,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>2020</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -197,8 +218,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>2021</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -214,25 +235,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>2022</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>75000</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>35000</v>
+        <v>40000</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>2023</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -242,48 +263,48 @@
         <v>40000</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
         <v>2024</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
         <v>2025</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
         <v>2026</v>
       </c>
       <c r="B9" s="0" t="n">
@@ -293,14 +314,14 @@
         <v>50000</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
         <v>2027</v>
       </c>
       <c r="B10" s="0" t="n">
@@ -310,14 +331,14 @@
         <v>50000</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
         <v>2028</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -327,14 +348,14 @@
         <v>50000</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>2029</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -344,14 +365,14 @@
         <v>50000</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>2030</v>
       </c>
       <c r="B13" s="0" t="n">
@@ -361,14 +382,14 @@
         <v>50000</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
         <v>2031</v>
       </c>
       <c r="B14" s="0" t="n">
@@ -378,14 +399,14 @@
         <v>50000</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
         <v>2032</v>
       </c>
       <c r="B15" s="0" t="n">
@@ -395,14 +416,14 @@
         <v>50000</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
         <v>2033</v>
       </c>
       <c r="B16" s="0" t="n">
@@ -412,14 +433,14 @@
         <v>50000</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
         <v>2034</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -429,14 +450,14 @@
         <v>50000</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
         <v>2035</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -446,14 +467,14 @@
         <v>50000</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
         <v>2036</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -463,14 +484,14 @@
         <v>50000</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
         <v>2037</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -480,14 +501,14 @@
         <v>50000</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
         <v>2038</v>
       </c>
       <c r="B21" s="0" t="n">
@@ -497,14 +518,14 @@
         <v>50000</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
         <v>2039</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -514,240 +535,733 @@
         <v>50000</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>7500</v>
+        <v>8000</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
         <v>2040</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
         <v>2041</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C24" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
         <v>2042</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C25" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
         <v>2043</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
         <v>2044</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
         <v>2045</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
         <v>2046</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
         <v>2047</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
         <v>2048</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
         <v>2049</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
         <v>2050</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
         <v>2051</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
         <v>2052</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>100000</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>7500</v>
+        <v>6000</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>2053</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>2054</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
+        <v>2055</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>2056</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>2057</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>4100</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>2058</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>4200</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>2059</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>4300</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>2060</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>4400</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>2061</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>4500</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>2062</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>4600</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>2063</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>4700</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
+        <v>2064</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="E47" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
+        <v>2065</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>4900</v>
+      </c>
+      <c r="E48" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>2066</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>2067</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>5100</v>
+      </c>
+      <c r="E50" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>2068</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>5200</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>2069</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>5300</v>
+      </c>
+      <c r="E52" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>2070</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>5400</v>
+      </c>
+      <c r="E53" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>2071</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>5500</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>2072</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>5600</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>2073</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>5700</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>2074</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>5800</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>2075</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>5900</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>2076</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>2077</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>6100</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>2078</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>6200</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>2079</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>6300</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>2080</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>6400</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>2081</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>6500</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added nudge for 10% expense reduction. Fixed previous bugs. PyFin seems to be working quite well, except that there seems to be a glitch with the pso.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -153,18 +153,18 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H58" activeCellId="0" sqref="H58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,7 +223,7 @@
         <v>2021</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>50000</v>
+        <v>38750</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>30000</v>
@@ -240,10 +240,10 @@
         <v>2022</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>75000</v>
+        <v>39750</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>40000</v>
+        <v>30001</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>6000</v>
@@ -257,10 +257,10 @@
         <v>2023</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>85000</v>
+        <v>40750</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>40000</v>
+        <v>30002</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>6000</v>
@@ -274,10 +274,10 @@
         <v>2024</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>100000</v>
+        <v>41750</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>40000</v>
+        <v>30003</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>6000</v>
@@ -291,10 +291,10 @@
         <v>2025</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>100000</v>
+        <v>42750</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>40000</v>
+        <v>30004</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>6000</v>
@@ -308,10 +308,10 @@
         <v>2026</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>100000</v>
+        <v>43750</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>50000</v>
+        <v>30005</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>8000</v>
@@ -325,10 +325,10 @@
         <v>2027</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>100000</v>
+        <v>44750</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>50000</v>
+        <v>30006</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>8000</v>
@@ -342,10 +342,10 @@
         <v>2028</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>100000</v>
+        <v>45750</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>50000</v>
+        <v>30007</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>8000</v>
@@ -359,10 +359,10 @@
         <v>2029</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>100000</v>
+        <v>46750</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>50000</v>
+        <v>30008</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>8000</v>
@@ -376,10 +376,10 @@
         <v>2030</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>100000</v>
+        <v>47750</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>50000</v>
+        <v>30009</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>8000</v>
@@ -393,10 +393,10 @@
         <v>2031</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>100000</v>
+        <v>48750</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>50000</v>
+        <v>30010</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>8000</v>
@@ -410,10 +410,10 @@
         <v>2032</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>100000</v>
+        <v>49750</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>50000</v>
+        <v>30011</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>8000</v>
@@ -427,10 +427,10 @@
         <v>2033</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>100000</v>
+        <v>50750</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>50000</v>
+        <v>30012</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>8000</v>
@@ -444,10 +444,10 @@
         <v>2034</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>100000</v>
+        <v>51750</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>50000</v>
+        <v>30013</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>8000</v>
@@ -461,10 +461,10 @@
         <v>2035</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>100000</v>
+        <v>52750</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>50000</v>
+        <v>30014</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>8000</v>
@@ -478,10 +478,10 @@
         <v>2036</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>100000</v>
+        <v>53750</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>50000</v>
+        <v>30015</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>8000</v>
@@ -495,10 +495,10 @@
         <v>2037</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>100000</v>
+        <v>54750</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>50000</v>
+        <v>30016</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>8000</v>
@@ -512,7 +512,7 @@
         <v>2038</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>100000</v>
+        <v>55750</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>50000</v>
@@ -529,7 +529,7 @@
         <v>2039</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>100000</v>
+        <v>56750</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>50000</v>
@@ -546,7 +546,7 @@
         <v>2040</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>100000</v>
+        <v>57750</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>40000</v>
@@ -563,7 +563,7 @@
         <v>2041</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>100000</v>
+        <v>58750</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>40000</v>
@@ -580,7 +580,7 @@
         <v>2042</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>100000</v>
+        <v>59750</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>40000</v>
@@ -597,7 +597,7 @@
         <v>2043</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>100000</v>
+        <v>60750</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>40000</v>
@@ -614,7 +614,7 @@
         <v>2044</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>100000</v>
+        <v>61750</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>40000</v>
@@ -631,7 +631,7 @@
         <v>2045</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>100000</v>
+        <v>62750</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>40000</v>
@@ -648,7 +648,7 @@
         <v>2046</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>100000</v>
+        <v>63750</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>40000</v>
@@ -665,7 +665,7 @@
         <v>2047</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>100000</v>
+        <v>64750</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>40000</v>
@@ -682,7 +682,7 @@
         <v>2048</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>100000</v>
+        <v>65750</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>40000</v>
@@ -699,7 +699,7 @@
         <v>2049</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>100000</v>
+        <v>66750</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>40000</v>
@@ -716,7 +716,7 @@
         <v>2050</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>100000</v>
+        <v>67750</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>40000</v>
@@ -733,7 +733,7 @@
         <v>2051</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>100000</v>
+        <v>68750</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>40000</v>
@@ -750,7 +750,7 @@
         <v>2052</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>100000</v>
+        <v>69750</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>40000</v>
@@ -1258,7 +1258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>